<commit_message>
fixed DV temp and updated report filters
</commit_message>
<xml_diff>
--- a/DV_temp.xlsx
+++ b/DV_temp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Streamlit_Projects\PIT 25\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{279D5419-5EFA-4198-9BBB-B9CE06339890}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCB59712-2DBB-419A-890D-1755C13D6BAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -490,13 +490,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="cell_style" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
@@ -803,7 +803,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F189"/>
   <sheetViews>
-    <sheetView topLeftCell="A177" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C146" sqref="C146:F188"/>
     </sheetView>
   </sheetViews>
@@ -816,14 +816,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
@@ -932,7 +932,7 @@
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -944,7 +944,7 @@
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="4"/>
+      <c r="A13" s="2"/>
       <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
@@ -954,7 +954,7 @@
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -966,7 +966,7 @@
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="4"/>
+      <c r="A15" s="2"/>
       <c r="B15" s="1" t="s">
         <v>19</v>
       </c>
@@ -976,7 +976,7 @@
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="4"/>
+      <c r="A16" s="2"/>
       <c r="B16" s="1" t="s">
         <v>20</v>
       </c>
@@ -986,7 +986,7 @@
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="4"/>
+      <c r="A17" s="2"/>
       <c r="B17" s="1" t="s">
         <v>21</v>
       </c>
@@ -996,7 +996,7 @@
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="4"/>
+      <c r="A18" s="2"/>
       <c r="B18" s="1" t="s">
         <v>22</v>
       </c>
@@ -1006,7 +1006,7 @@
       <c r="F18" s="1"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="4"/>
+      <c r="A19" s="2"/>
       <c r="B19" s="1" t="s">
         <v>23</v>
       </c>
@@ -1016,7 +1016,7 @@
       <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="4"/>
+      <c r="A20" s="2"/>
       <c r="B20" s="1" t="s">
         <v>24</v>
       </c>
@@ -1026,7 +1026,7 @@
       <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="4"/>
+      <c r="A21" s="2"/>
       <c r="B21" s="1" t="s">
         <v>25</v>
       </c>
@@ -1036,7 +1036,7 @@
       <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="4"/>
+      <c r="A22" s="2"/>
       <c r="B22" s="1" t="s">
         <v>26</v>
       </c>
@@ -1046,7 +1046,7 @@
       <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="4"/>
+      <c r="A23" s="2"/>
       <c r="B23" s="1" t="s">
         <v>27</v>
       </c>
@@ -1056,7 +1056,7 @@
       <c r="F23" s="1"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="4"/>
+      <c r="A24" s="2"/>
       <c r="B24" s="1" t="s">
         <v>28</v>
       </c>
@@ -1066,7 +1066,7 @@
       <c r="F24" s="1"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="4"/>
+      <c r="A25" s="2"/>
       <c r="B25" s="1" t="s">
         <v>29</v>
       </c>
@@ -1076,7 +1076,7 @@
       <c r="F25" s="1"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="4"/>
+      <c r="A26" s="2"/>
       <c r="B26" s="1" t="s">
         <v>30</v>
       </c>
@@ -1086,7 +1086,7 @@
       <c r="F26" s="1"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="4"/>
+      <c r="A27" s="2"/>
       <c r="B27" s="1" t="s">
         <v>31</v>
       </c>
@@ -1096,7 +1096,7 @@
       <c r="F27" s="1"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="4"/>
+      <c r="A28" s="2"/>
       <c r="B28" s="1" t="s">
         <v>32</v>
       </c>
@@ -1106,7 +1106,7 @@
       <c r="F28" s="1"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -1118,7 +1118,7 @@
       <c r="F29" s="1"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="4"/>
+      <c r="A30" s="2"/>
       <c r="B30" s="1" t="s">
         <v>35</v>
       </c>
@@ -1128,7 +1128,7 @@
       <c r="F30" s="1"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="4"/>
+      <c r="A31" s="2"/>
       <c r="B31" s="1" t="s">
         <v>36</v>
       </c>
@@ -1138,7 +1138,7 @@
       <c r="F31" s="1"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="4"/>
+      <c r="A32" s="2"/>
       <c r="B32" s="1" t="s">
         <v>37</v>
       </c>
@@ -1148,7 +1148,7 @@
       <c r="F32" s="1"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="4"/>
+      <c r="A33" s="2"/>
       <c r="B33" s="1" t="s">
         <v>38</v>
       </c>
@@ -1158,7 +1158,7 @@
       <c r="F33" s="1"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="4"/>
+      <c r="A34" s="2"/>
       <c r="B34" s="1" t="s">
         <v>39</v>
       </c>
@@ -1168,7 +1168,7 @@
       <c r="F34" s="1"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" s="4"/>
+      <c r="A35" s="2"/>
       <c r="B35" s="1" t="s">
         <v>40</v>
       </c>
@@ -1178,7 +1178,7 @@
       <c r="F35" s="1"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="4"/>
+      <c r="A36" s="2"/>
       <c r="B36" s="1" t="s">
         <v>41</v>
       </c>
@@ -1188,7 +1188,7 @@
       <c r="F36" s="1"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="4"/>
+      <c r="A37" s="2"/>
       <c r="B37" s="1" t="s">
         <v>42</v>
       </c>
@@ -1198,7 +1198,7 @@
       <c r="F37" s="1"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="4"/>
+      <c r="A38" s="2"/>
       <c r="B38" s="1" t="s">
         <v>43</v>
       </c>
@@ -1208,7 +1208,7 @@
       <c r="F38" s="1"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="4"/>
+      <c r="A39" s="2"/>
       <c r="B39" s="1" t="s">
         <v>44</v>
       </c>
@@ -1218,7 +1218,7 @@
       <c r="F39" s="1"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="4"/>
+      <c r="A40" s="2"/>
       <c r="B40" s="1" t="s">
         <v>45</v>
       </c>
@@ -1228,7 +1228,7 @@
       <c r="F40" s="1"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" s="4"/>
+      <c r="A41" s="2"/>
       <c r="B41" s="1" t="s">
         <v>46</v>
       </c>
@@ -1238,7 +1238,7 @@
       <c r="F41" s="1"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" s="4"/>
+      <c r="A42" s="2"/>
       <c r="B42" s="1" t="s">
         <v>47</v>
       </c>
@@ -1248,7 +1248,7 @@
       <c r="F42" s="1"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="4"/>
+      <c r="A43" s="2"/>
       <c r="B43" s="1" t="s">
         <v>48</v>
       </c>
@@ -1258,7 +1258,7 @@
       <c r="F43" s="1"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" s="4" t="s">
+      <c r="A44" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B44" s="1" t="s">
@@ -1270,7 +1270,7 @@
       <c r="F44" s="1"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" s="4"/>
+      <c r="A45" s="2"/>
       <c r="B45" s="1" t="s">
         <v>50</v>
       </c>
@@ -1288,14 +1288,14 @@
       <c r="F46" s="1"/>
     </row>
     <row r="52" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A52" s="2" t="s">
+      <c r="A52" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B52" s="3"/>
-      <c r="C52" s="3"/>
-      <c r="D52" s="3"/>
-      <c r="E52" s="3"/>
-      <c r="F52" s="3"/>
+      <c r="B52" s="4"/>
+      <c r="C52" s="4"/>
+      <c r="D52" s="4"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="1"/>
@@ -1394,7 +1394,7 @@
       <c r="F61" s="1"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A62" s="4" t="s">
+      <c r="A62" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B62" s="1" t="s">
@@ -1406,7 +1406,7 @@
       <c r="F62" s="1"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A63" s="4"/>
+      <c r="A63" s="2"/>
       <c r="B63" s="1" t="s">
         <v>16</v>
       </c>
@@ -1416,7 +1416,7 @@
       <c r="F63" s="1"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A64" s="4" t="s">
+      <c r="A64" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B64" s="1" t="s">
@@ -1428,7 +1428,7 @@
       <c r="F64" s="1"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A65" s="4"/>
+      <c r="A65" s="2"/>
       <c r="B65" s="1" t="s">
         <v>19</v>
       </c>
@@ -1438,7 +1438,7 @@
       <c r="F65" s="1"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A66" s="4"/>
+      <c r="A66" s="2"/>
       <c r="B66" s="1" t="s">
         <v>20</v>
       </c>
@@ -1448,7 +1448,7 @@
       <c r="F66" s="1"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A67" s="4"/>
+      <c r="A67" s="2"/>
       <c r="B67" s="1" t="s">
         <v>21</v>
       </c>
@@ -1458,7 +1458,7 @@
       <c r="F67" s="1"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A68" s="4"/>
+      <c r="A68" s="2"/>
       <c r="B68" s="1" t="s">
         <v>22</v>
       </c>
@@ -1468,7 +1468,7 @@
       <c r="F68" s="1"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A69" s="4"/>
+      <c r="A69" s="2"/>
       <c r="B69" s="1" t="s">
         <v>23</v>
       </c>
@@ -1478,7 +1478,7 @@
       <c r="F69" s="1"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A70" s="4"/>
+      <c r="A70" s="2"/>
       <c r="B70" s="1" t="s">
         <v>24</v>
       </c>
@@ -1488,7 +1488,7 @@
       <c r="F70" s="1"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A71" s="4"/>
+      <c r="A71" s="2"/>
       <c r="B71" s="1" t="s">
         <v>25</v>
       </c>
@@ -1498,7 +1498,7 @@
       <c r="F71" s="1"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A72" s="4"/>
+      <c r="A72" s="2"/>
       <c r="B72" s="1" t="s">
         <v>26</v>
       </c>
@@ -1508,7 +1508,7 @@
       <c r="F72" s="1"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A73" s="4"/>
+      <c r="A73" s="2"/>
       <c r="B73" s="1" t="s">
         <v>27</v>
       </c>
@@ -1518,7 +1518,7 @@
       <c r="F73" s="1"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A74" s="4"/>
+      <c r="A74" s="2"/>
       <c r="B74" s="1" t="s">
         <v>28</v>
       </c>
@@ -1528,7 +1528,7 @@
       <c r="F74" s="1"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A75" s="4"/>
+      <c r="A75" s="2"/>
       <c r="B75" s="1" t="s">
         <v>29</v>
       </c>
@@ -1538,7 +1538,7 @@
       <c r="F75" s="1"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A76" s="4"/>
+      <c r="A76" s="2"/>
       <c r="B76" s="1" t="s">
         <v>30</v>
       </c>
@@ -1548,7 +1548,7 @@
       <c r="F76" s="1"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A77" s="4"/>
+      <c r="A77" s="2"/>
       <c r="B77" s="1" t="s">
         <v>31</v>
       </c>
@@ -1558,7 +1558,7 @@
       <c r="F77" s="1"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A78" s="4"/>
+      <c r="A78" s="2"/>
       <c r="B78" s="1" t="s">
         <v>32</v>
       </c>
@@ -1568,7 +1568,7 @@
       <c r="F78" s="1"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A79" s="4" t="s">
+      <c r="A79" s="2" t="s">
         <v>54</v>
       </c>
       <c r="B79" s="1" t="s">
@@ -1580,7 +1580,7 @@
       <c r="F79" s="1"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A80" s="4"/>
+      <c r="A80" s="2"/>
       <c r="B80" s="1" t="s">
         <v>35</v>
       </c>
@@ -1590,7 +1590,7 @@
       <c r="F80" s="1"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A81" s="4"/>
+      <c r="A81" s="2"/>
       <c r="B81" s="1" t="s">
         <v>36</v>
       </c>
@@ -1600,7 +1600,7 @@
       <c r="F81" s="1"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A82" s="4"/>
+      <c r="A82" s="2"/>
       <c r="B82" s="1" t="s">
         <v>37</v>
       </c>
@@ -1610,7 +1610,7 @@
       <c r="F82" s="1"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A83" s="4"/>
+      <c r="A83" s="2"/>
       <c r="B83" s="1" t="s">
         <v>38</v>
       </c>
@@ -1620,7 +1620,7 @@
       <c r="F83" s="1"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A84" s="4"/>
+      <c r="A84" s="2"/>
       <c r="B84" s="1" t="s">
         <v>39</v>
       </c>
@@ -1630,7 +1630,7 @@
       <c r="F84" s="1"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A85" s="4"/>
+      <c r="A85" s="2"/>
       <c r="B85" s="1" t="s">
         <v>40</v>
       </c>
@@ -1640,7 +1640,7 @@
       <c r="F85" s="1"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A86" s="4"/>
+      <c r="A86" s="2"/>
       <c r="B86" s="1" t="s">
         <v>41</v>
       </c>
@@ -1650,7 +1650,7 @@
       <c r="F86" s="1"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A87" s="4"/>
+      <c r="A87" s="2"/>
       <c r="B87" s="1" t="s">
         <v>42</v>
       </c>
@@ -1660,7 +1660,7 @@
       <c r="F87" s="1"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A88" s="4"/>
+      <c r="A88" s="2"/>
       <c r="B88" s="1" t="s">
         <v>43</v>
       </c>
@@ -1670,7 +1670,7 @@
       <c r="F88" s="1"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A89" s="4"/>
+      <c r="A89" s="2"/>
       <c r="B89" s="1" t="s">
         <v>44</v>
       </c>
@@ -1680,7 +1680,7 @@
       <c r="F89" s="1"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A90" s="4"/>
+      <c r="A90" s="2"/>
       <c r="B90" s="1" t="s">
         <v>45</v>
       </c>
@@ -1690,7 +1690,7 @@
       <c r="F90" s="1"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A91" s="4"/>
+      <c r="A91" s="2"/>
       <c r="B91" s="1" t="s">
         <v>46</v>
       </c>
@@ -1700,7 +1700,7 @@
       <c r="F91" s="1"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A92" s="4"/>
+      <c r="A92" s="2"/>
       <c r="B92" s="1" t="s">
         <v>47</v>
       </c>
@@ -1710,7 +1710,7 @@
       <c r="F92" s="1"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A93" s="4"/>
+      <c r="A93" s="2"/>
       <c r="B93" s="1" t="s">
         <v>48</v>
       </c>
@@ -1740,14 +1740,14 @@
       <c r="F95" s="1"/>
     </row>
     <row r="101" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A101" s="2" t="s">
+      <c r="A101" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B101" s="3"/>
-      <c r="C101" s="3"/>
-      <c r="D101" s="3"/>
-      <c r="E101" s="3"/>
-      <c r="F101" s="3"/>
+      <c r="B101" s="4"/>
+      <c r="C101" s="4"/>
+      <c r="D101" s="4"/>
+      <c r="E101" s="4"/>
+      <c r="F101" s="4"/>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102" s="1"/>
@@ -1786,7 +1786,7 @@
       <c r="F104" s="1"/>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A105" s="4" t="s">
+      <c r="A105" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B105" s="1" t="s">
@@ -1798,7 +1798,7 @@
       <c r="F105" s="1"/>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A106" s="4"/>
+      <c r="A106" s="2"/>
       <c r="B106" s="1" t="s">
         <v>16</v>
       </c>
@@ -1808,7 +1808,7 @@
       <c r="F106" s="1"/>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A107" s="4" t="s">
+      <c r="A107" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B107" s="1" t="s">
@@ -1820,7 +1820,7 @@
       <c r="F107" s="1"/>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A108" s="4"/>
+      <c r="A108" s="2"/>
       <c r="B108" s="1" t="s">
         <v>19</v>
       </c>
@@ -1830,7 +1830,7 @@
       <c r="F108" s="1"/>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A109" s="4"/>
+      <c r="A109" s="2"/>
       <c r="B109" s="1" t="s">
         <v>20</v>
       </c>
@@ -1840,7 +1840,7 @@
       <c r="F109" s="1"/>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A110" s="4"/>
+      <c r="A110" s="2"/>
       <c r="B110" s="1" t="s">
         <v>21</v>
       </c>
@@ -1850,7 +1850,7 @@
       <c r="F110" s="1"/>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A111" s="4"/>
+      <c r="A111" s="2"/>
       <c r="B111" s="1" t="s">
         <v>22</v>
       </c>
@@ -1860,7 +1860,7 @@
       <c r="F111" s="1"/>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A112" s="4"/>
+      <c r="A112" s="2"/>
       <c r="B112" s="1" t="s">
         <v>23</v>
       </c>
@@ -1870,7 +1870,7 @@
       <c r="F112" s="1"/>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A113" s="4"/>
+      <c r="A113" s="2"/>
       <c r="B113" s="1" t="s">
         <v>24</v>
       </c>
@@ -1880,7 +1880,7 @@
       <c r="F113" s="1"/>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A114" s="4"/>
+      <c r="A114" s="2"/>
       <c r="B114" s="1" t="s">
         <v>25</v>
       </c>
@@ -1890,7 +1890,7 @@
       <c r="F114" s="1"/>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A115" s="4"/>
+      <c r="A115" s="2"/>
       <c r="B115" s="1" t="s">
         <v>26</v>
       </c>
@@ -1900,7 +1900,7 @@
       <c r="F115" s="1"/>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A116" s="4"/>
+      <c r="A116" s="2"/>
       <c r="B116" s="1" t="s">
         <v>27</v>
       </c>
@@ -1910,7 +1910,7 @@
       <c r="F116" s="1"/>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A117" s="4"/>
+      <c r="A117" s="2"/>
       <c r="B117" s="1" t="s">
         <v>28</v>
       </c>
@@ -1920,7 +1920,7 @@
       <c r="F117" s="1"/>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A118" s="4"/>
+      <c r="A118" s="2"/>
       <c r="B118" s="1" t="s">
         <v>29</v>
       </c>
@@ -1930,7 +1930,7 @@
       <c r="F118" s="1"/>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A119" s="4"/>
+      <c r="A119" s="2"/>
       <c r="B119" s="1" t="s">
         <v>30</v>
       </c>
@@ -1940,7 +1940,7 @@
       <c r="F119" s="1"/>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A120" s="4"/>
+      <c r="A120" s="2"/>
       <c r="B120" s="1" t="s">
         <v>31</v>
       </c>
@@ -1950,7 +1950,7 @@
       <c r="F120" s="1"/>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A121" s="4"/>
+      <c r="A121" s="2"/>
       <c r="B121" s="1" t="s">
         <v>32</v>
       </c>
@@ -1960,7 +1960,7 @@
       <c r="F121" s="1"/>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A122" s="4" t="s">
+      <c r="A122" s="2" t="s">
         <v>54</v>
       </c>
       <c r="B122" s="1" t="s">
@@ -1972,7 +1972,7 @@
       <c r="F122" s="1"/>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A123" s="4"/>
+      <c r="A123" s="2"/>
       <c r="B123" s="1" t="s">
         <v>35</v>
       </c>
@@ -1982,7 +1982,7 @@
       <c r="F123" s="1"/>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A124" s="4"/>
+      <c r="A124" s="2"/>
       <c r="B124" s="1" t="s">
         <v>36</v>
       </c>
@@ -1992,7 +1992,7 @@
       <c r="F124" s="1"/>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A125" s="4"/>
+      <c r="A125" s="2"/>
       <c r="B125" s="1" t="s">
         <v>37</v>
       </c>
@@ -2002,7 +2002,7 @@
       <c r="F125" s="1"/>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A126" s="4"/>
+      <c r="A126" s="2"/>
       <c r="B126" s="1" t="s">
         <v>38</v>
       </c>
@@ -2012,7 +2012,7 @@
       <c r="F126" s="1"/>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A127" s="4"/>
+      <c r="A127" s="2"/>
       <c r="B127" s="1" t="s">
         <v>39</v>
       </c>
@@ -2022,7 +2022,7 @@
       <c r="F127" s="1"/>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A128" s="4"/>
+      <c r="A128" s="2"/>
       <c r="B128" s="1" t="s">
         <v>40</v>
       </c>
@@ -2032,7 +2032,7 @@
       <c r="F128" s="1"/>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A129" s="4"/>
+      <c r="A129" s="2"/>
       <c r="B129" s="1" t="s">
         <v>41</v>
       </c>
@@ -2042,7 +2042,7 @@
       <c r="F129" s="1"/>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A130" s="4"/>
+      <c r="A130" s="2"/>
       <c r="B130" s="1" t="s">
         <v>42</v>
       </c>
@@ -2052,7 +2052,7 @@
       <c r="F130" s="1"/>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A131" s="4"/>
+      <c r="A131" s="2"/>
       <c r="B131" s="1" t="s">
         <v>43</v>
       </c>
@@ -2062,7 +2062,7 @@
       <c r="F131" s="1"/>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A132" s="4"/>
+      <c r="A132" s="2"/>
       <c r="B132" s="1" t="s">
         <v>44</v>
       </c>
@@ -2072,7 +2072,7 @@
       <c r="F132" s="1"/>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A133" s="4"/>
+      <c r="A133" s="2"/>
       <c r="B133" s="1" t="s">
         <v>45</v>
       </c>
@@ -2082,7 +2082,7 @@
       <c r="F133" s="1"/>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A134" s="4"/>
+      <c r="A134" s="2"/>
       <c r="B134" s="1" t="s">
         <v>46</v>
       </c>
@@ -2092,7 +2092,7 @@
       <c r="F134" s="1"/>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A135" s="4"/>
+      <c r="A135" s="2"/>
       <c r="B135" s="1" t="s">
         <v>47</v>
       </c>
@@ -2102,7 +2102,7 @@
       <c r="F135" s="1"/>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A136" s="4"/>
+      <c r="A136" s="2"/>
       <c r="B136" s="1" t="s">
         <v>48</v>
       </c>
@@ -2132,14 +2132,14 @@
       <c r="F138" s="1"/>
     </row>
     <row r="144" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A144" s="2" t="s">
+      <c r="A144" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B144" s="3"/>
-      <c r="C144" s="3"/>
-      <c r="D144" s="3"/>
-      <c r="E144" s="3"/>
-      <c r="F144" s="3"/>
+      <c r="B144" s="4"/>
+      <c r="C144" s="4"/>
+      <c r="D144" s="4"/>
+      <c r="E144" s="4"/>
+      <c r="F144" s="4"/>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A145" s="1"/>
@@ -2248,7 +2248,7 @@
       <c r="F154" s="1"/>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A155" s="4" t="s">
+      <c r="A155" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B155" s="1" t="s">
@@ -2260,7 +2260,7 @@
       <c r="F155" s="1"/>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A156" s="4"/>
+      <c r="A156" s="2"/>
       <c r="B156" s="1" t="s">
         <v>16</v>
       </c>
@@ -2270,7 +2270,7 @@
       <c r="F156" s="1"/>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A157" s="4" t="s">
+      <c r="A157" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B157" s="1" t="s">
@@ -2282,7 +2282,7 @@
       <c r="F157" s="1"/>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A158" s="4"/>
+      <c r="A158" s="2"/>
       <c r="B158" s="1" t="s">
         <v>19</v>
       </c>
@@ -2292,7 +2292,7 @@
       <c r="F158" s="1"/>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A159" s="4"/>
+      <c r="A159" s="2"/>
       <c r="B159" s="1" t="s">
         <v>20</v>
       </c>
@@ -2302,7 +2302,7 @@
       <c r="F159" s="1"/>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A160" s="4"/>
+      <c r="A160" s="2"/>
       <c r="B160" s="1" t="s">
         <v>21</v>
       </c>
@@ -2312,7 +2312,7 @@
       <c r="F160" s="1"/>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A161" s="4"/>
+      <c r="A161" s="2"/>
       <c r="B161" s="1" t="s">
         <v>22</v>
       </c>
@@ -2322,7 +2322,7 @@
       <c r="F161" s="1"/>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A162" s="4"/>
+      <c r="A162" s="2"/>
       <c r="B162" s="1" t="s">
         <v>23</v>
       </c>
@@ -2332,7 +2332,7 @@
       <c r="F162" s="1"/>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A163" s="4"/>
+      <c r="A163" s="2"/>
       <c r="B163" s="1" t="s">
         <v>24</v>
       </c>
@@ -2342,7 +2342,7 @@
       <c r="F163" s="1"/>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A164" s="4"/>
+      <c r="A164" s="2"/>
       <c r="B164" s="1" t="s">
         <v>25</v>
       </c>
@@ -2352,7 +2352,7 @@
       <c r="F164" s="1"/>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A165" s="4"/>
+      <c r="A165" s="2"/>
       <c r="B165" s="1" t="s">
         <v>26</v>
       </c>
@@ -2362,7 +2362,7 @@
       <c r="F165" s="1"/>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A166" s="4"/>
+      <c r="A166" s="2"/>
       <c r="B166" s="1" t="s">
         <v>27</v>
       </c>
@@ -2372,7 +2372,7 @@
       <c r="F166" s="1"/>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A167" s="4"/>
+      <c r="A167" s="2"/>
       <c r="B167" s="1" t="s">
         <v>28</v>
       </c>
@@ -2382,7 +2382,7 @@
       <c r="F167" s="1"/>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A168" s="4"/>
+      <c r="A168" s="2"/>
       <c r="B168" s="1" t="s">
         <v>29</v>
       </c>
@@ -2392,7 +2392,7 @@
       <c r="F168" s="1"/>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A169" s="4"/>
+      <c r="A169" s="2"/>
       <c r="B169" s="1" t="s">
         <v>30</v>
       </c>
@@ -2402,7 +2402,7 @@
       <c r="F169" s="1"/>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A170" s="4"/>
+      <c r="A170" s="2"/>
       <c r="B170" s="1" t="s">
         <v>31</v>
       </c>
@@ -2412,7 +2412,7 @@
       <c r="F170" s="1"/>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A171" s="4"/>
+      <c r="A171" s="2"/>
       <c r="B171" s="1" t="s">
         <v>32</v>
       </c>
@@ -2422,7 +2422,7 @@
       <c r="F171" s="1"/>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A172" s="4" t="s">
+      <c r="A172" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B172" s="1" t="s">
@@ -2434,7 +2434,7 @@
       <c r="F172" s="1"/>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A173" s="4"/>
+      <c r="A173" s="2"/>
       <c r="B173" s="1" t="s">
         <v>35</v>
       </c>
@@ -2444,7 +2444,7 @@
       <c r="F173" s="1"/>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A174" s="4"/>
+      <c r="A174" s="2"/>
       <c r="B174" s="1" t="s">
         <v>36</v>
       </c>
@@ -2454,7 +2454,7 @@
       <c r="F174" s="1"/>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A175" s="4"/>
+      <c r="A175" s="2"/>
       <c r="B175" s="1" t="s">
         <v>37</v>
       </c>
@@ -2464,7 +2464,7 @@
       <c r="F175" s="1"/>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A176" s="4"/>
+      <c r="A176" s="2"/>
       <c r="B176" s="1" t="s">
         <v>38</v>
       </c>
@@ -2474,7 +2474,7 @@
       <c r="F176" s="1"/>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A177" s="4"/>
+      <c r="A177" s="2"/>
       <c r="B177" s="1" t="s">
         <v>39</v>
       </c>
@@ -2484,7 +2484,7 @@
       <c r="F177" s="1"/>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A178" s="4"/>
+      <c r="A178" s="2"/>
       <c r="B178" s="1" t="s">
         <v>40</v>
       </c>
@@ -2494,7 +2494,7 @@
       <c r="F178" s="1"/>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A179" s="4"/>
+      <c r="A179" s="2"/>
       <c r="B179" s="1" t="s">
         <v>41</v>
       </c>
@@ -2504,7 +2504,7 @@
       <c r="F179" s="1"/>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A180" s="4"/>
+      <c r="A180" s="2"/>
       <c r="B180" s="1" t="s">
         <v>42</v>
       </c>
@@ -2514,7 +2514,7 @@
       <c r="F180" s="1"/>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A181" s="4"/>
+      <c r="A181" s="2"/>
       <c r="B181" s="1" t="s">
         <v>43</v>
       </c>
@@ -2524,7 +2524,7 @@
       <c r="F181" s="1"/>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A182" s="4"/>
+      <c r="A182" s="2"/>
       <c r="B182" s="1" t="s">
         <v>44</v>
       </c>
@@ -2534,7 +2534,7 @@
       <c r="F182" s="1"/>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A183" s="4"/>
+      <c r="A183" s="2"/>
       <c r="B183" s="1" t="s">
         <v>45</v>
       </c>
@@ -2544,7 +2544,7 @@
       <c r="F183" s="1"/>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A184" s="4"/>
+      <c r="A184" s="2"/>
       <c r="B184" s="1" t="s">
         <v>46</v>
       </c>
@@ -2554,7 +2554,7 @@
       <c r="F184" s="1"/>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A185" s="4"/>
+      <c r="A185" s="2"/>
       <c r="B185" s="1" t="s">
         <v>47</v>
       </c>
@@ -2564,7 +2564,7 @@
       <c r="F185" s="1"/>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A186" s="4"/>
+      <c r="A186" s="2"/>
       <c r="B186" s="1" t="s">
         <v>48</v>
       </c>
@@ -2574,7 +2574,7 @@
       <c r="F186" s="1"/>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A187" s="4" t="s">
+      <c r="A187" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B187" s="1" t="s">
@@ -2586,7 +2586,7 @@
       <c r="F187" s="1"/>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A188" s="4"/>
+      <c r="A188" s="2"/>
       <c r="B188" s="1" t="s">
         <v>50</v>
       </c>
@@ -2605,6 +2605,8 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A172:A186"/>
+    <mergeCell ref="A12:A13"/>
     <mergeCell ref="A79:A93"/>
     <mergeCell ref="A157:A171"/>
     <mergeCell ref="A1:F1"/>
@@ -2621,8 +2623,6 @@
     <mergeCell ref="A155:A156"/>
     <mergeCell ref="A52:F52"/>
     <mergeCell ref="A29:A43"/>
-    <mergeCell ref="A172:A186"/>
-    <mergeCell ref="A12:A13"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -2632,8 +2632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F129"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48:F83"/>
+    <sheetView topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="C92" sqref="C92:F128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2645,14 +2645,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
@@ -2701,7 +2701,7 @@
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="2" t="s">
         <v>60</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -2713,7 +2713,7 @@
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="4"/>
+      <c r="A7" s="2"/>
       <c r="B7" s="1" t="s">
         <v>16</v>
       </c>
@@ -2723,7 +2723,7 @@
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="2" t="s">
         <v>61</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -2735,7 +2735,7 @@
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="4"/>
+      <c r="A9" s="2"/>
       <c r="B9" s="1" t="s">
         <v>19</v>
       </c>
@@ -2745,7 +2745,7 @@
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="4"/>
+      <c r="A10" s="2"/>
       <c r="B10" s="1" t="s">
         <v>20</v>
       </c>
@@ -2755,7 +2755,7 @@
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
+      <c r="A11" s="2"/>
       <c r="B11" s="1" t="s">
         <v>21</v>
       </c>
@@ -2765,7 +2765,7 @@
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="4"/>
+      <c r="A12" s="2"/>
       <c r="B12" s="1" t="s">
         <v>22</v>
       </c>
@@ -2775,7 +2775,7 @@
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="4"/>
+      <c r="A13" s="2"/>
       <c r="B13" s="1" t="s">
         <v>23</v>
       </c>
@@ -2785,7 +2785,7 @@
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="4"/>
+      <c r="A14" s="2"/>
       <c r="B14" s="1" t="s">
         <v>24</v>
       </c>
@@ -2795,7 +2795,7 @@
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="4"/>
+      <c r="A15" s="2"/>
       <c r="B15" s="1" t="s">
         <v>25</v>
       </c>
@@ -2805,7 +2805,7 @@
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="4"/>
+      <c r="A16" s="2"/>
       <c r="B16" s="1" t="s">
         <v>26</v>
       </c>
@@ -2815,7 +2815,7 @@
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="4"/>
+      <c r="A17" s="2"/>
       <c r="B17" s="1" t="s">
         <v>27</v>
       </c>
@@ -2825,7 +2825,7 @@
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="4"/>
+      <c r="A18" s="2"/>
       <c r="B18" s="1" t="s">
         <v>28</v>
       </c>
@@ -2835,7 +2835,7 @@
       <c r="F18" s="1"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="4"/>
+      <c r="A19" s="2"/>
       <c r="B19" s="1" t="s">
         <v>29</v>
       </c>
@@ -2845,7 +2845,7 @@
       <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="4"/>
+      <c r="A20" s="2"/>
       <c r="B20" s="1" t="s">
         <v>30</v>
       </c>
@@ -2855,7 +2855,7 @@
       <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="4"/>
+      <c r="A21" s="2"/>
       <c r="B21" s="1" t="s">
         <v>31</v>
       </c>
@@ -2865,7 +2865,7 @@
       <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="4"/>
+      <c r="A22" s="2"/>
       <c r="B22" s="1" t="s">
         <v>32</v>
       </c>
@@ -2875,7 +2875,7 @@
       <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="2" t="s">
         <v>62</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -2887,7 +2887,7 @@
       <c r="F23" s="1"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="4"/>
+      <c r="A24" s="2"/>
       <c r="B24" s="1" t="s">
         <v>35</v>
       </c>
@@ -2897,7 +2897,7 @@
       <c r="F24" s="1"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="4"/>
+      <c r="A25" s="2"/>
       <c r="B25" s="1" t="s">
         <v>36</v>
       </c>
@@ -2907,7 +2907,7 @@
       <c r="F25" s="1"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="4"/>
+      <c r="A26" s="2"/>
       <c r="B26" s="1" t="s">
         <v>37</v>
       </c>
@@ -2917,7 +2917,7 @@
       <c r="F26" s="1"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="4"/>
+      <c r="A27" s="2"/>
       <c r="B27" s="1" t="s">
         <v>38</v>
       </c>
@@ -2927,7 +2927,7 @@
       <c r="F27" s="1"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="4"/>
+      <c r="A28" s="2"/>
       <c r="B28" s="1" t="s">
         <v>39</v>
       </c>
@@ -2937,7 +2937,7 @@
       <c r="F28" s="1"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="4"/>
+      <c r="A29" s="2"/>
       <c r="B29" s="1" t="s">
         <v>40</v>
       </c>
@@ -2947,7 +2947,7 @@
       <c r="F29" s="1"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="4"/>
+      <c r="A30" s="2"/>
       <c r="B30" s="1" t="s">
         <v>41</v>
       </c>
@@ -2957,7 +2957,7 @@
       <c r="F30" s="1"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="4"/>
+      <c r="A31" s="2"/>
       <c r="B31" s="1" t="s">
         <v>42</v>
       </c>
@@ -2967,7 +2967,7 @@
       <c r="F31" s="1"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="4"/>
+      <c r="A32" s="2"/>
       <c r="B32" s="1" t="s">
         <v>43</v>
       </c>
@@ -2977,7 +2977,7 @@
       <c r="F32" s="1"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="4"/>
+      <c r="A33" s="2"/>
       <c r="B33" s="1" t="s">
         <v>44</v>
       </c>
@@ -2987,7 +2987,7 @@
       <c r="F33" s="1"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="4"/>
+      <c r="A34" s="2"/>
       <c r="B34" s="1" t="s">
         <v>45</v>
       </c>
@@ -2997,7 +2997,7 @@
       <c r="F34" s="1"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" s="4"/>
+      <c r="A35" s="2"/>
       <c r="B35" s="1" t="s">
         <v>46</v>
       </c>
@@ -3007,7 +3007,7 @@
       <c r="F35" s="1"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="4"/>
+      <c r="A36" s="2"/>
       <c r="B36" s="1" t="s">
         <v>47</v>
       </c>
@@ -3017,7 +3017,7 @@
       <c r="F36" s="1"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="4"/>
+      <c r="A37" s="2"/>
       <c r="B37" s="1" t="s">
         <v>48</v>
       </c>
@@ -3027,7 +3027,7 @@
       <c r="F37" s="1"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="4" t="s">
+      <c r="A38" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -3039,7 +3039,7 @@
       <c r="F38" s="1"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="4"/>
+      <c r="A39" s="2"/>
       <c r="B39" s="1" t="s">
         <v>50</v>
       </c>
@@ -3057,14 +3057,14 @@
       <c r="F40" s="1"/>
     </row>
     <row r="46" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A46" s="2" t="s">
+      <c r="A46" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
@@ -3113,7 +3113,7 @@
       <c r="F50" s="1"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" s="4" t="s">
+      <c r="A51" s="2" t="s">
         <v>60</v>
       </c>
       <c r="B51" s="1" t="s">
@@ -3125,7 +3125,7 @@
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" s="4"/>
+      <c r="A52" s="2"/>
       <c r="B52" s="1" t="s">
         <v>16</v>
       </c>
@@ -3135,7 +3135,7 @@
       <c r="F52" s="1"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53" s="4" t="s">
+      <c r="A53" s="2" t="s">
         <v>61</v>
       </c>
       <c r="B53" s="1" t="s">
@@ -3147,7 +3147,7 @@
       <c r="F53" s="1"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A54" s="4"/>
+      <c r="A54" s="2"/>
       <c r="B54" s="1" t="s">
         <v>19</v>
       </c>
@@ -3157,7 +3157,7 @@
       <c r="F54" s="1"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A55" s="4"/>
+      <c r="A55" s="2"/>
       <c r="B55" s="1" t="s">
         <v>20</v>
       </c>
@@ -3167,7 +3167,7 @@
       <c r="F55" s="1"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A56" s="4"/>
+      <c r="A56" s="2"/>
       <c r="B56" s="1" t="s">
         <v>21</v>
       </c>
@@ -3177,7 +3177,7 @@
       <c r="F56" s="1"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A57" s="4"/>
+      <c r="A57" s="2"/>
       <c r="B57" s="1" t="s">
         <v>22</v>
       </c>
@@ -3187,7 +3187,7 @@
       <c r="F57" s="1"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A58" s="4"/>
+      <c r="A58" s="2"/>
       <c r="B58" s="1" t="s">
         <v>23</v>
       </c>
@@ -3197,7 +3197,7 @@
       <c r="F58" s="1"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59" s="4"/>
+      <c r="A59" s="2"/>
       <c r="B59" s="1" t="s">
         <v>24</v>
       </c>
@@ -3207,7 +3207,7 @@
       <c r="F59" s="1"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A60" s="4"/>
+      <c r="A60" s="2"/>
       <c r="B60" s="1" t="s">
         <v>25</v>
       </c>
@@ -3217,7 +3217,7 @@
       <c r="F60" s="1"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A61" s="4"/>
+      <c r="A61" s="2"/>
       <c r="B61" s="1" t="s">
         <v>26</v>
       </c>
@@ -3227,7 +3227,7 @@
       <c r="F61" s="1"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A62" s="4"/>
+      <c r="A62" s="2"/>
       <c r="B62" s="1" t="s">
         <v>27</v>
       </c>
@@ -3237,7 +3237,7 @@
       <c r="F62" s="1"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A63" s="4"/>
+      <c r="A63" s="2"/>
       <c r="B63" s="1" t="s">
         <v>28</v>
       </c>
@@ -3247,7 +3247,7 @@
       <c r="F63" s="1"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A64" s="4"/>
+      <c r="A64" s="2"/>
       <c r="B64" s="1" t="s">
         <v>29</v>
       </c>
@@ -3257,7 +3257,7 @@
       <c r="F64" s="1"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A65" s="4"/>
+      <c r="A65" s="2"/>
       <c r="B65" s="1" t="s">
         <v>30</v>
       </c>
@@ -3267,7 +3267,7 @@
       <c r="F65" s="1"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A66" s="4"/>
+      <c r="A66" s="2"/>
       <c r="B66" s="1" t="s">
         <v>31</v>
       </c>
@@ -3277,7 +3277,7 @@
       <c r="F66" s="1"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A67" s="4"/>
+      <c r="A67" s="2"/>
       <c r="B67" s="1" t="s">
         <v>32</v>
       </c>
@@ -3287,7 +3287,7 @@
       <c r="F67" s="1"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A68" s="4" t="s">
+      <c r="A68" s="2" t="s">
         <v>62</v>
       </c>
       <c r="B68" s="1" t="s">
@@ -3299,7 +3299,7 @@
       <c r="F68" s="1"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A69" s="4"/>
+      <c r="A69" s="2"/>
       <c r="B69" s="1" t="s">
         <v>35</v>
       </c>
@@ -3309,7 +3309,7 @@
       <c r="F69" s="1"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A70" s="4"/>
+      <c r="A70" s="2"/>
       <c r="B70" s="1" t="s">
         <v>36</v>
       </c>
@@ -3319,7 +3319,7 @@
       <c r="F70" s="1"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A71" s="4"/>
+      <c r="A71" s="2"/>
       <c r="B71" s="1" t="s">
         <v>37</v>
       </c>
@@ -3329,7 +3329,7 @@
       <c r="F71" s="1"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A72" s="4"/>
+      <c r="A72" s="2"/>
       <c r="B72" s="1" t="s">
         <v>38</v>
       </c>
@@ -3339,7 +3339,7 @@
       <c r="F72" s="1"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A73" s="4"/>
+      <c r="A73" s="2"/>
       <c r="B73" s="1" t="s">
         <v>39</v>
       </c>
@@ -3349,7 +3349,7 @@
       <c r="F73" s="1"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A74" s="4"/>
+      <c r="A74" s="2"/>
       <c r="B74" s="1" t="s">
         <v>40</v>
       </c>
@@ -3359,7 +3359,7 @@
       <c r="F74" s="1"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A75" s="4"/>
+      <c r="A75" s="2"/>
       <c r="B75" s="1" t="s">
         <v>41</v>
       </c>
@@ -3369,7 +3369,7 @@
       <c r="F75" s="1"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A76" s="4"/>
+      <c r="A76" s="2"/>
       <c r="B76" s="1" t="s">
         <v>42</v>
       </c>
@@ -3379,7 +3379,7 @@
       <c r="F76" s="1"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A77" s="4"/>
+      <c r="A77" s="2"/>
       <c r="B77" s="1" t="s">
         <v>43</v>
       </c>
@@ -3389,7 +3389,7 @@
       <c r="F77" s="1"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A78" s="4"/>
+      <c r="A78" s="2"/>
       <c r="B78" s="1" t="s">
         <v>44</v>
       </c>
@@ -3399,7 +3399,7 @@
       <c r="F78" s="1"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A79" s="4"/>
+      <c r="A79" s="2"/>
       <c r="B79" s="1" t="s">
         <v>45</v>
       </c>
@@ -3409,7 +3409,7 @@
       <c r="F79" s="1"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A80" s="4"/>
+      <c r="A80" s="2"/>
       <c r="B80" s="1" t="s">
         <v>46</v>
       </c>
@@ -3419,7 +3419,7 @@
       <c r="F80" s="1"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A81" s="4"/>
+      <c r="A81" s="2"/>
       <c r="B81" s="1" t="s">
         <v>47</v>
       </c>
@@ -3429,7 +3429,7 @@
       <c r="F81" s="1"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A82" s="4"/>
+      <c r="A82" s="2"/>
       <c r="B82" s="1" t="s">
         <v>48</v>
       </c>
@@ -3459,14 +3459,14 @@
       <c r="F84" s="1"/>
     </row>
     <row r="90" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A90" s="2" t="s">
+      <c r="A90" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B90" s="3"/>
-      <c r="C90" s="3"/>
-      <c r="D90" s="3"/>
-      <c r="E90" s="3"/>
-      <c r="F90" s="3"/>
+      <c r="B90" s="4"/>
+      <c r="C90" s="4"/>
+      <c r="D90" s="4"/>
+      <c r="E90" s="4"/>
+      <c r="F90" s="4"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" s="1"/>
@@ -3489,674 +3489,378 @@
         <v>5</v>
       </c>
       <c r="B92" s="1"/>
-      <c r="C92" s="1">
-        <v>5</v>
-      </c>
-      <c r="D92" s="1">
-        <v>1</v>
-      </c>
-      <c r="E92" s="1">
-        <v>16</v>
-      </c>
-      <c r="F92" s="1">
-        <v>22</v>
-      </c>
+      <c r="C92" s="1"/>
+      <c r="D92" s="1"/>
+      <c r="E92" s="1"/>
+      <c r="F92" s="1"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B93" s="1"/>
-      <c r="C93" s="1">
-        <v>6</v>
-      </c>
-      <c r="D93" s="1">
-        <v>2</v>
-      </c>
-      <c r="E93" s="1">
-        <v>23</v>
-      </c>
-      <c r="F93" s="1">
-        <v>31</v>
-      </c>
+      <c r="C93" s="1"/>
+      <c r="D93" s="1"/>
+      <c r="E93" s="1"/>
+      <c r="F93" s="1"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B94" s="1"/>
-      <c r="C94" s="1">
-        <v>5</v>
-      </c>
-      <c r="D94" s="1">
-        <v>1</v>
-      </c>
-      <c r="E94" s="1">
-        <v>16</v>
-      </c>
-      <c r="F94" s="1">
-        <v>22</v>
-      </c>
+      <c r="C94" s="1"/>
+      <c r="D94" s="1"/>
+      <c r="E94" s="1"/>
+      <c r="F94" s="1"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A95" s="4" t="s">
+      <c r="A95" s="2" t="s">
         <v>60</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C95" s="1">
-        <v>0</v>
-      </c>
-      <c r="D95" s="1">
-        <v>0</v>
-      </c>
-      <c r="E95" s="1">
-        <v>0</v>
-      </c>
-      <c r="F95" s="1">
-        <v>0</v>
-      </c>
+      <c r="C95" s="1"/>
+      <c r="D95" s="1"/>
+      <c r="E95" s="1"/>
+      <c r="F95" s="1"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A96" s="4"/>
+      <c r="A96" s="2"/>
       <c r="B96" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C96" s="1">
-        <v>0</v>
-      </c>
-      <c r="D96" s="1">
-        <v>0</v>
-      </c>
-      <c r="E96" s="1">
-        <v>0</v>
-      </c>
-      <c r="F96" s="1">
-        <v>0</v>
-      </c>
+      <c r="C96" s="1"/>
+      <c r="D96" s="1"/>
+      <c r="E96" s="1"/>
+      <c r="F96" s="1"/>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A97" s="4" t="s">
+      <c r="A97" s="2" t="s">
         <v>61</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C97" s="1">
-        <v>1</v>
-      </c>
-      <c r="D97" s="1">
-        <v>1</v>
-      </c>
-      <c r="E97" s="1">
-        <v>3</v>
-      </c>
-      <c r="F97" s="1">
-        <v>5</v>
-      </c>
+      <c r="C97" s="1"/>
+      <c r="D97" s="1"/>
+      <c r="E97" s="1"/>
+      <c r="F97" s="1"/>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A98" s="4"/>
+      <c r="A98" s="2"/>
       <c r="B98" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C98" s="1">
-        <v>3</v>
-      </c>
-      <c r="D98" s="1">
-        <v>0</v>
-      </c>
-      <c r="E98" s="1">
-        <v>13</v>
-      </c>
-      <c r="F98" s="1">
-        <v>16</v>
-      </c>
+      <c r="C98" s="1"/>
+      <c r="D98" s="1"/>
+      <c r="E98" s="1"/>
+      <c r="F98" s="1"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A99" s="4"/>
+      <c r="A99" s="2"/>
       <c r="B99" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C99" s="1">
-        <v>0</v>
-      </c>
-      <c r="D99" s="1">
-        <v>0</v>
-      </c>
-      <c r="E99" s="1">
-        <v>0</v>
-      </c>
-      <c r="F99" s="1">
-        <v>0</v>
-      </c>
+      <c r="C99" s="1"/>
+      <c r="D99" s="1"/>
+      <c r="E99" s="1"/>
+      <c r="F99" s="1"/>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A100" s="4"/>
+      <c r="A100" s="2"/>
       <c r="B100" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C100" s="1">
-        <v>0</v>
-      </c>
-      <c r="D100" s="1">
-        <v>0</v>
-      </c>
-      <c r="E100" s="1">
-        <v>0</v>
-      </c>
-      <c r="F100" s="1">
-        <v>0</v>
-      </c>
+      <c r="C100" s="1"/>
+      <c r="D100" s="1"/>
+      <c r="E100" s="1"/>
+      <c r="F100" s="1"/>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A101" s="4"/>
+      <c r="A101" s="2"/>
       <c r="B101" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C101" s="1">
-        <v>1</v>
-      </c>
-      <c r="D101" s="1">
-        <v>0</v>
-      </c>
-      <c r="E101" s="1">
-        <v>0</v>
-      </c>
-      <c r="F101" s="1">
-        <v>1</v>
-      </c>
+      <c r="C101" s="1"/>
+      <c r="D101" s="1"/>
+      <c r="E101" s="1"/>
+      <c r="F101" s="1"/>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A102" s="4"/>
+      <c r="A102" s="2"/>
       <c r="B102" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C102" s="1">
-        <v>0</v>
-      </c>
-      <c r="D102" s="1">
-        <v>0</v>
-      </c>
-      <c r="E102" s="1">
-        <v>0</v>
-      </c>
-      <c r="F102" s="1">
-        <v>0</v>
-      </c>
+      <c r="C102" s="1"/>
+      <c r="D102" s="1"/>
+      <c r="E102" s="1"/>
+      <c r="F102" s="1"/>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A103" s="4"/>
+      <c r="A103" s="2"/>
       <c r="B103" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C103" s="1">
-        <v>0</v>
-      </c>
-      <c r="D103" s="1">
-        <v>0</v>
-      </c>
-      <c r="E103" s="1">
-        <v>0</v>
-      </c>
-      <c r="F103" s="1">
-        <v>0</v>
-      </c>
+      <c r="C103" s="1"/>
+      <c r="D103" s="1"/>
+      <c r="E103" s="1"/>
+      <c r="F103" s="1"/>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A104" s="4"/>
+      <c r="A104" s="2"/>
       <c r="B104" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C104" s="1">
-        <v>0</v>
-      </c>
-      <c r="D104" s="1">
-        <v>0</v>
-      </c>
-      <c r="E104" s="1">
-        <v>0</v>
-      </c>
-      <c r="F104" s="1">
-        <v>0</v>
-      </c>
+      <c r="C104" s="1"/>
+      <c r="D104" s="1"/>
+      <c r="E104" s="1"/>
+      <c r="F104" s="1"/>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A105" s="4"/>
+      <c r="A105" s="2"/>
       <c r="B105" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C105" s="1">
-        <v>0</v>
-      </c>
-      <c r="D105" s="1">
-        <v>0</v>
-      </c>
-      <c r="E105" s="1">
-        <v>0</v>
-      </c>
-      <c r="F105" s="1">
-        <v>0</v>
-      </c>
+      <c r="C105" s="1"/>
+      <c r="D105" s="1"/>
+      <c r="E105" s="1"/>
+      <c r="F105" s="1"/>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A106" s="4"/>
+      <c r="A106" s="2"/>
       <c r="B106" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C106" s="1">
-        <v>0</v>
-      </c>
-      <c r="D106" s="1">
-        <v>0</v>
-      </c>
-      <c r="E106" s="1">
-        <v>0</v>
-      </c>
-      <c r="F106" s="1">
-        <v>0</v>
-      </c>
+      <c r="C106" s="1"/>
+      <c r="D106" s="1"/>
+      <c r="E106" s="1"/>
+      <c r="F106" s="1"/>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A107" s="4"/>
+      <c r="A107" s="2"/>
       <c r="B107" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C107" s="1">
-        <v>0</v>
-      </c>
-      <c r="D107" s="1">
-        <v>0</v>
-      </c>
-      <c r="E107" s="1">
-        <v>0</v>
-      </c>
-      <c r="F107" s="1">
-        <v>0</v>
-      </c>
+      <c r="C107" s="1"/>
+      <c r="D107" s="1"/>
+      <c r="E107" s="1"/>
+      <c r="F107" s="1"/>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A108" s="4"/>
+      <c r="A108" s="2"/>
       <c r="B108" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C108" s="1">
-        <v>0</v>
-      </c>
-      <c r="D108" s="1">
-        <v>0</v>
-      </c>
-      <c r="E108" s="1">
-        <v>0</v>
-      </c>
-      <c r="F108" s="1">
-        <v>0</v>
-      </c>
+      <c r="C108" s="1"/>
+      <c r="D108" s="1"/>
+      <c r="E108" s="1"/>
+      <c r="F108" s="1"/>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A109" s="4"/>
+      <c r="A109" s="2"/>
       <c r="B109" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C109" s="1">
-        <v>0</v>
-      </c>
-      <c r="D109" s="1">
-        <v>0</v>
-      </c>
-      <c r="E109" s="1">
-        <v>0</v>
-      </c>
-      <c r="F109" s="1">
-        <v>0</v>
-      </c>
+      <c r="C109" s="1"/>
+      <c r="D109" s="1"/>
+      <c r="E109" s="1"/>
+      <c r="F109" s="1"/>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A110" s="4"/>
+      <c r="A110" s="2"/>
       <c r="B110" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C110" s="1">
-        <v>0</v>
-      </c>
-      <c r="D110" s="1">
-        <v>0</v>
-      </c>
-      <c r="E110" s="1">
-        <v>0</v>
-      </c>
-      <c r="F110" s="1">
-        <v>0</v>
-      </c>
+      <c r="C110" s="1"/>
+      <c r="D110" s="1"/>
+      <c r="E110" s="1"/>
+      <c r="F110" s="1"/>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A111" s="4"/>
+      <c r="A111" s="2"/>
       <c r="B111" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C111" s="1">
-        <v>0</v>
-      </c>
-      <c r="D111" s="1">
-        <v>0</v>
-      </c>
-      <c r="E111" s="1">
-        <v>0</v>
-      </c>
-      <c r="F111" s="1">
-        <v>0</v>
-      </c>
+      <c r="C111" s="1"/>
+      <c r="D111" s="1"/>
+      <c r="E111" s="1"/>
+      <c r="F111" s="1"/>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A112" s="4" t="s">
+      <c r="A112" s="2" t="s">
         <v>62</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C112" s="1">
-        <v>0</v>
-      </c>
-      <c r="D112" s="1">
-        <v>0</v>
-      </c>
-      <c r="E112" s="1">
-        <v>0</v>
-      </c>
-      <c r="F112" s="1">
-        <v>0</v>
-      </c>
+      <c r="C112" s="1"/>
+      <c r="D112" s="1"/>
+      <c r="E112" s="1"/>
+      <c r="F112" s="1"/>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A113" s="4"/>
+      <c r="A113" s="2"/>
       <c r="B113" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C113" s="1">
-        <v>0</v>
-      </c>
-      <c r="D113" s="1">
-        <v>0</v>
-      </c>
-      <c r="E113" s="1">
-        <v>0</v>
-      </c>
-      <c r="F113" s="1">
-        <v>0</v>
-      </c>
+      <c r="C113" s="1"/>
+      <c r="D113" s="1"/>
+      <c r="E113" s="1"/>
+      <c r="F113" s="1"/>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A114" s="4"/>
+      <c r="A114" s="2"/>
       <c r="B114" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C114" s="1">
-        <v>0</v>
-      </c>
-      <c r="D114" s="1">
-        <v>0</v>
-      </c>
-      <c r="E114" s="1">
-        <v>0</v>
-      </c>
-      <c r="F114" s="1">
-        <v>0</v>
-      </c>
+      <c r="C114" s="1"/>
+      <c r="D114" s="1"/>
+      <c r="E114" s="1"/>
+      <c r="F114" s="1"/>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A115" s="4"/>
+      <c r="A115" s="2"/>
       <c r="B115" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C115" s="1">
-        <v>0</v>
-      </c>
-      <c r="D115" s="1">
-        <v>0</v>
-      </c>
-      <c r="E115" s="1">
-        <v>0</v>
-      </c>
-      <c r="F115" s="1">
-        <v>0</v>
-      </c>
+      <c r="C115" s="1"/>
+      <c r="D115" s="1"/>
+      <c r="E115" s="1"/>
+      <c r="F115" s="1"/>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A116" s="4"/>
+      <c r="A116" s="2"/>
       <c r="B116" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C116" s="1">
-        <v>0</v>
-      </c>
-      <c r="D116" s="1">
-        <v>0</v>
-      </c>
-      <c r="E116" s="1">
-        <v>0</v>
-      </c>
-      <c r="F116" s="1">
-        <v>0</v>
-      </c>
+      <c r="C116" s="1"/>
+      <c r="D116" s="1"/>
+      <c r="E116" s="1"/>
+      <c r="F116" s="1"/>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A117" s="4"/>
+      <c r="A117" s="2"/>
       <c r="B117" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C117" s="1">
-        <v>0</v>
-      </c>
-      <c r="D117" s="1">
-        <v>0</v>
-      </c>
-      <c r="E117" s="1">
-        <v>0</v>
-      </c>
-      <c r="F117" s="1">
-        <v>0</v>
-      </c>
+      <c r="C117" s="1"/>
+      <c r="D117" s="1"/>
+      <c r="E117" s="1"/>
+      <c r="F117" s="1"/>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A118" s="4"/>
+      <c r="A118" s="2"/>
       <c r="B118" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C118" s="1">
-        <v>0</v>
-      </c>
-      <c r="D118" s="1">
-        <v>0</v>
-      </c>
-      <c r="E118" s="1">
-        <v>1</v>
-      </c>
-      <c r="F118" s="1">
-        <v>1</v>
-      </c>
+      <c r="C118" s="1"/>
+      <c r="D118" s="1"/>
+      <c r="E118" s="1"/>
+      <c r="F118" s="1"/>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A119" s="4"/>
+      <c r="A119" s="2"/>
       <c r="B119" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C119" s="1">
-        <v>0</v>
-      </c>
-      <c r="D119" s="1">
-        <v>0</v>
-      </c>
-      <c r="E119" s="1">
-        <v>0</v>
-      </c>
-      <c r="F119" s="1">
-        <v>0</v>
-      </c>
+      <c r="C119" s="1"/>
+      <c r="D119" s="1"/>
+      <c r="E119" s="1"/>
+      <c r="F119" s="1"/>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A120" s="4"/>
+      <c r="A120" s="2"/>
       <c r="B120" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C120" s="1">
-        <v>0</v>
-      </c>
-      <c r="D120" s="1">
-        <v>0</v>
-      </c>
-      <c r="E120" s="1">
-        <v>0</v>
-      </c>
-      <c r="F120" s="1">
-        <v>0</v>
-      </c>
+      <c r="C120" s="1"/>
+      <c r="D120" s="1"/>
+      <c r="E120" s="1"/>
+      <c r="F120" s="1"/>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A121" s="4"/>
+      <c r="A121" s="2"/>
       <c r="B121" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C121" s="1">
-        <v>0</v>
-      </c>
-      <c r="D121" s="1">
-        <v>0</v>
-      </c>
-      <c r="E121" s="1">
-        <v>0</v>
-      </c>
-      <c r="F121" s="1">
-        <v>0</v>
-      </c>
+      <c r="C121" s="1"/>
+      <c r="D121" s="1"/>
+      <c r="E121" s="1"/>
+      <c r="F121" s="1"/>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A122" s="4"/>
+      <c r="A122" s="2"/>
       <c r="B122" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C122" s="1">
-        <v>0</v>
-      </c>
-      <c r="D122" s="1">
-        <v>0</v>
-      </c>
-      <c r="E122" s="1">
-        <v>0</v>
-      </c>
-      <c r="F122" s="1">
-        <v>0</v>
-      </c>
+      <c r="C122" s="1"/>
+      <c r="D122" s="1"/>
+      <c r="E122" s="1"/>
+      <c r="F122" s="1"/>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A123" s="4"/>
+      <c r="A123" s="2"/>
       <c r="B123" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C123" s="1">
-        <v>5</v>
-      </c>
-      <c r="D123" s="1">
-        <v>1</v>
-      </c>
-      <c r="E123" s="1">
-        <v>15</v>
-      </c>
-      <c r="F123" s="1">
-        <v>21</v>
-      </c>
+      <c r="C123" s="1"/>
+      <c r="D123" s="1"/>
+      <c r="E123" s="1"/>
+      <c r="F123" s="1"/>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A124" s="4"/>
+      <c r="A124" s="2"/>
       <c r="B124" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C124" s="1">
-        <v>0</v>
-      </c>
-      <c r="D124" s="1">
-        <v>0</v>
-      </c>
-      <c r="E124" s="1">
-        <v>0</v>
-      </c>
-      <c r="F124" s="1">
-        <v>0</v>
-      </c>
+      <c r="C124" s="1"/>
+      <c r="D124" s="1"/>
+      <c r="E124" s="1"/>
+      <c r="F124" s="1"/>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A125" s="4"/>
+      <c r="A125" s="2"/>
       <c r="B125" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C125" s="1">
-        <v>0</v>
-      </c>
-      <c r="D125" s="1">
-        <v>0</v>
-      </c>
-      <c r="E125" s="1">
-        <v>0</v>
-      </c>
-      <c r="F125" s="1">
-        <v>0</v>
-      </c>
+      <c r="C125" s="1"/>
+      <c r="D125" s="1"/>
+      <c r="E125" s="1"/>
+      <c r="F125" s="1"/>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A126" s="4"/>
+      <c r="A126" s="2"/>
       <c r="B126" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C126" s="1">
-        <v>0</v>
-      </c>
-      <c r="D126" s="1">
-        <v>0</v>
-      </c>
-      <c r="E126" s="1">
-        <v>0</v>
-      </c>
-      <c r="F126" s="1">
-        <v>0</v>
-      </c>
+      <c r="C126" s="1"/>
+      <c r="D126" s="1"/>
+      <c r="E126" s="1"/>
+      <c r="F126" s="1"/>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A127" s="4" t="s">
+      <c r="A127" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B127" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C127" s="1">
-        <v>1</v>
-      </c>
-      <c r="D127" s="1">
-        <v>0</v>
-      </c>
-      <c r="E127" s="1">
-        <v>9</v>
-      </c>
-      <c r="F127" s="1">
-        <v>10</v>
-      </c>
+      <c r="C127" s="1"/>
+      <c r="D127" s="1"/>
+      <c r="E127" s="1"/>
+      <c r="F127" s="1"/>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A128" s="4"/>
+      <c r="A128" s="2"/>
       <c r="B128" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C128" s="1">
-        <v>1</v>
-      </c>
-      <c r="D128" s="1">
-        <v>0</v>
-      </c>
-      <c r="E128" s="1">
-        <v>14</v>
-      </c>
-      <c r="F128" s="1">
-        <v>15</v>
-      </c>
+      <c r="C128" s="1"/>
+      <c r="D128" s="1"/>
+      <c r="E128" s="1"/>
+      <c r="F128" s="1"/>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A129" s="1"/>
@@ -4204,14 +3908,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
@@ -4270,7 +3974,7 @@
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -4282,7 +3986,7 @@
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="4"/>
+      <c r="A8" s="2"/>
       <c r="B8" s="1" t="s">
         <v>16</v>
       </c>
@@ -4292,7 +3996,7 @@
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="2" t="s">
         <v>71</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -4304,7 +4008,7 @@
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="4"/>
+      <c r="A10" s="2"/>
       <c r="B10" s="1" t="s">
         <v>19</v>
       </c>
@@ -4314,7 +4018,7 @@
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
+      <c r="A11" s="2"/>
       <c r="B11" s="1" t="s">
         <v>20</v>
       </c>
@@ -4324,7 +4028,7 @@
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="4"/>
+      <c r="A12" s="2"/>
       <c r="B12" s="1" t="s">
         <v>21</v>
       </c>
@@ -4334,7 +4038,7 @@
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="4"/>
+      <c r="A13" s="2"/>
       <c r="B13" s="1" t="s">
         <v>22</v>
       </c>
@@ -4344,7 +4048,7 @@
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="4"/>
+      <c r="A14" s="2"/>
       <c r="B14" s="1" t="s">
         <v>23</v>
       </c>
@@ -4354,7 +4058,7 @@
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="4"/>
+      <c r="A15" s="2"/>
       <c r="B15" s="1" t="s">
         <v>24</v>
       </c>
@@ -4364,7 +4068,7 @@
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="4"/>
+      <c r="A16" s="2"/>
       <c r="B16" s="1" t="s">
         <v>25</v>
       </c>
@@ -4374,7 +4078,7 @@
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="4"/>
+      <c r="A17" s="2"/>
       <c r="B17" s="1" t="s">
         <v>26</v>
       </c>
@@ -4384,7 +4088,7 @@
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="4"/>
+      <c r="A18" s="2"/>
       <c r="B18" s="1" t="s">
         <v>27</v>
       </c>
@@ -4394,7 +4098,7 @@
       <c r="F18" s="1"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="4"/>
+      <c r="A19" s="2"/>
       <c r="B19" s="1" t="s">
         <v>28</v>
       </c>
@@ -4404,7 +4108,7 @@
       <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="4"/>
+      <c r="A20" s="2"/>
       <c r="B20" s="1" t="s">
         <v>29</v>
       </c>
@@ -4414,7 +4118,7 @@
       <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="4"/>
+      <c r="A21" s="2"/>
       <c r="B21" s="1" t="s">
         <v>30</v>
       </c>
@@ -4424,7 +4128,7 @@
       <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="4"/>
+      <c r="A22" s="2"/>
       <c r="B22" s="1" t="s">
         <v>31</v>
       </c>
@@ -4434,7 +4138,7 @@
       <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="4"/>
+      <c r="A23" s="2"/>
       <c r="B23" s="1" t="s">
         <v>32</v>
       </c>
@@ -4444,7 +4148,7 @@
       <c r="F23" s="1"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="2" t="s">
         <v>72</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -4456,7 +4160,7 @@
       <c r="F24" s="1"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="4"/>
+      <c r="A25" s="2"/>
       <c r="B25" s="1" t="s">
         <v>35</v>
       </c>
@@ -4466,7 +4170,7 @@
       <c r="F25" s="1"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="4"/>
+      <c r="A26" s="2"/>
       <c r="B26" s="1" t="s">
         <v>36</v>
       </c>
@@ -4476,7 +4180,7 @@
       <c r="F26" s="1"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="4"/>
+      <c r="A27" s="2"/>
       <c r="B27" s="1" t="s">
         <v>37</v>
       </c>
@@ -4486,7 +4190,7 @@
       <c r="F27" s="1"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="4"/>
+      <c r="A28" s="2"/>
       <c r="B28" s="1" t="s">
         <v>38</v>
       </c>
@@ -4496,7 +4200,7 @@
       <c r="F28" s="1"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="4"/>
+      <c r="A29" s="2"/>
       <c r="B29" s="1" t="s">
         <v>39</v>
       </c>
@@ -4506,7 +4210,7 @@
       <c r="F29" s="1"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="4"/>
+      <c r="A30" s="2"/>
       <c r="B30" s="1" t="s">
         <v>40</v>
       </c>
@@ -4516,7 +4220,7 @@
       <c r="F30" s="1"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="4"/>
+      <c r="A31" s="2"/>
       <c r="B31" s="1" t="s">
         <v>41</v>
       </c>
@@ -4526,7 +4230,7 @@
       <c r="F31" s="1"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="4"/>
+      <c r="A32" s="2"/>
       <c r="B32" s="1" t="s">
         <v>42</v>
       </c>
@@ -4536,7 +4240,7 @@
       <c r="F32" s="1"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="4"/>
+      <c r="A33" s="2"/>
       <c r="B33" s="1" t="s">
         <v>43</v>
       </c>
@@ -4546,7 +4250,7 @@
       <c r="F33" s="1"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="4"/>
+      <c r="A34" s="2"/>
       <c r="B34" s="1" t="s">
         <v>44</v>
       </c>
@@ -4556,7 +4260,7 @@
       <c r="F34" s="1"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" s="4"/>
+      <c r="A35" s="2"/>
       <c r="B35" s="1" t="s">
         <v>45</v>
       </c>
@@ -4566,7 +4270,7 @@
       <c r="F35" s="1"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="4"/>
+      <c r="A36" s="2"/>
       <c r="B36" s="1" t="s">
         <v>46</v>
       </c>
@@ -4576,7 +4280,7 @@
       <c r="F36" s="1"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="4"/>
+      <c r="A37" s="2"/>
       <c r="B37" s="1" t="s">
         <v>47</v>
       </c>
@@ -4586,7 +4290,7 @@
       <c r="F37" s="1"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="4"/>
+      <c r="A38" s="2"/>
       <c r="B38" s="1" t="s">
         <v>48</v>
       </c>
@@ -4616,14 +4320,14 @@
       <c r="F40" s="1"/>
     </row>
     <row r="46" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A46" s="2" t="s">
+      <c r="A46" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
@@ -4722,7 +4426,7 @@
       <c r="F55" s="1"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A56" s="4" t="s">
+      <c r="A56" s="2" t="s">
         <v>82</v>
       </c>
       <c r="B56" s="1" t="s">
@@ -4734,7 +4438,7 @@
       <c r="F56" s="1"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A57" s="4"/>
+      <c r="A57" s="2"/>
       <c r="B57" s="1" t="s">
         <v>16</v>
       </c>
@@ -4744,7 +4448,7 @@
       <c r="F57" s="1"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A58" s="4" t="s">
+      <c r="A58" s="2" t="s">
         <v>83</v>
       </c>
       <c r="B58" s="1" t="s">
@@ -4756,7 +4460,7 @@
       <c r="F58" s="1"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59" s="4"/>
+      <c r="A59" s="2"/>
       <c r="B59" s="1" t="s">
         <v>19</v>
       </c>
@@ -4766,7 +4470,7 @@
       <c r="F59" s="1"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A60" s="4"/>
+      <c r="A60" s="2"/>
       <c r="B60" s="1" t="s">
         <v>20</v>
       </c>
@@ -4776,7 +4480,7 @@
       <c r="F60" s="1"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A61" s="4"/>
+      <c r="A61" s="2"/>
       <c r="B61" s="1" t="s">
         <v>21</v>
       </c>
@@ -4786,7 +4490,7 @@
       <c r="F61" s="1"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A62" s="4"/>
+      <c r="A62" s="2"/>
       <c r="B62" s="1" t="s">
         <v>22</v>
       </c>
@@ -4796,7 +4500,7 @@
       <c r="F62" s="1"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A63" s="4"/>
+      <c r="A63" s="2"/>
       <c r="B63" s="1" t="s">
         <v>23</v>
       </c>
@@ -4806,7 +4510,7 @@
       <c r="F63" s="1"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A64" s="4"/>
+      <c r="A64" s="2"/>
       <c r="B64" s="1" t="s">
         <v>24</v>
       </c>
@@ -4816,7 +4520,7 @@
       <c r="F64" s="1"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A65" s="4"/>
+      <c r="A65" s="2"/>
       <c r="B65" s="1" t="s">
         <v>25</v>
       </c>
@@ -4826,7 +4530,7 @@
       <c r="F65" s="1"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A66" s="4"/>
+      <c r="A66" s="2"/>
       <c r="B66" s="1" t="s">
         <v>26</v>
       </c>
@@ -4836,7 +4540,7 @@
       <c r="F66" s="1"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A67" s="4"/>
+      <c r="A67" s="2"/>
       <c r="B67" s="1" t="s">
         <v>27</v>
       </c>
@@ -4846,7 +4550,7 @@
       <c r="F67" s="1"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A68" s="4"/>
+      <c r="A68" s="2"/>
       <c r="B68" s="1" t="s">
         <v>28</v>
       </c>
@@ -4856,7 +4560,7 @@
       <c r="F68" s="1"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A69" s="4"/>
+      <c r="A69" s="2"/>
       <c r="B69" s="1" t="s">
         <v>29</v>
       </c>
@@ -4866,7 +4570,7 @@
       <c r="F69" s="1"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A70" s="4"/>
+      <c r="A70" s="2"/>
       <c r="B70" s="1" t="s">
         <v>30</v>
       </c>
@@ -4876,7 +4580,7 @@
       <c r="F70" s="1"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A71" s="4"/>
+      <c r="A71" s="2"/>
       <c r="B71" s="1" t="s">
         <v>31</v>
       </c>
@@ -4886,7 +4590,7 @@
       <c r="F71" s="1"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A72" s="4"/>
+      <c r="A72" s="2"/>
       <c r="B72" s="1" t="s">
         <v>32</v>
       </c>
@@ -4896,7 +4600,7 @@
       <c r="F72" s="1"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A73" s="4" t="s">
+      <c r="A73" s="2" t="s">
         <v>84</v>
       </c>
       <c r="B73" s="1" t="s">
@@ -4908,7 +4612,7 @@
       <c r="F73" s="1"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A74" s="4"/>
+      <c r="A74" s="2"/>
       <c r="B74" s="1" t="s">
         <v>35</v>
       </c>
@@ -4918,7 +4622,7 @@
       <c r="F74" s="1"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A75" s="4"/>
+      <c r="A75" s="2"/>
       <c r="B75" s="1" t="s">
         <v>36</v>
       </c>
@@ -4928,7 +4632,7 @@
       <c r="F75" s="1"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A76" s="4"/>
+      <c r="A76" s="2"/>
       <c r="B76" s="1" t="s">
         <v>37</v>
       </c>
@@ -4938,7 +4642,7 @@
       <c r="F76" s="1"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A77" s="4"/>
+      <c r="A77" s="2"/>
       <c r="B77" s="1" t="s">
         <v>38</v>
       </c>
@@ -4948,7 +4652,7 @@
       <c r="F77" s="1"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A78" s="4"/>
+      <c r="A78" s="2"/>
       <c r="B78" s="1" t="s">
         <v>39</v>
       </c>
@@ -4958,7 +4662,7 @@
       <c r="F78" s="1"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A79" s="4"/>
+      <c r="A79" s="2"/>
       <c r="B79" s="1" t="s">
         <v>40</v>
       </c>
@@ -4968,7 +4672,7 @@
       <c r="F79" s="1"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A80" s="4"/>
+      <c r="A80" s="2"/>
       <c r="B80" s="1" t="s">
         <v>41</v>
       </c>
@@ -4978,7 +4682,7 @@
       <c r="F80" s="1"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A81" s="4"/>
+      <c r="A81" s="2"/>
       <c r="B81" s="1" t="s">
         <v>42</v>
       </c>
@@ -4988,7 +4692,7 @@
       <c r="F81" s="1"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A82" s="4"/>
+      <c r="A82" s="2"/>
       <c r="B82" s="1" t="s">
         <v>43</v>
       </c>
@@ -4998,7 +4702,7 @@
       <c r="F82" s="1"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A83" s="4"/>
+      <c r="A83" s="2"/>
       <c r="B83" s="1" t="s">
         <v>44</v>
       </c>
@@ -5008,7 +4712,7 @@
       <c r="F83" s="1"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A84" s="4"/>
+      <c r="A84" s="2"/>
       <c r="B84" s="1" t="s">
         <v>45</v>
       </c>
@@ -5018,7 +4722,7 @@
       <c r="F84" s="1"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A85" s="4"/>
+      <c r="A85" s="2"/>
       <c r="B85" s="1" t="s">
         <v>46</v>
       </c>
@@ -5028,7 +4732,7 @@
       <c r="F85" s="1"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A86" s="4"/>
+      <c r="A86" s="2"/>
       <c r="B86" s="1" t="s">
         <v>47</v>
       </c>
@@ -5038,7 +4742,7 @@
       <c r="F86" s="1"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A87" s="4"/>
+      <c r="A87" s="2"/>
       <c r="B87" s="1" t="s">
         <v>48</v>
       </c>
@@ -5048,7 +4752,7 @@
       <c r="F87" s="1"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A88" s="4" t="s">
+      <c r="A88" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B88" s="1" t="s">
@@ -5060,7 +4764,7 @@
       <c r="F88" s="1"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A89" s="4"/>
+      <c r="A89" s="2"/>
       <c r="B89" s="1" t="s">
         <v>50</v>
       </c>
@@ -5111,14 +4815,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
@@ -5210,14 +4914,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
@@ -5236,7 +4940,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="1"/>
@@ -5246,7 +4950,7 @@
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="4"/>
+      <c r="A4" s="2"/>
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -5256,7 +4960,7 @@
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="4"/>
+      <c r="A5" s="2"/>
       <c r="B5" s="1" t="s">
         <v>91</v>
       </c>
@@ -5266,7 +4970,7 @@
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="4"/>
+      <c r="A6" s="2"/>
       <c r="B6" s="1" t="s">
         <v>92</v>
       </c>
@@ -5276,7 +4980,7 @@
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="4"/>
+      <c r="A7" s="2"/>
       <c r="B7" s="1" t="s">
         <v>93</v>
       </c>
@@ -5286,7 +4990,7 @@
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="4"/>
+      <c r="A8" s="2"/>
       <c r="B8" s="1" t="s">
         <v>94</v>
       </c>
@@ -5296,7 +5000,7 @@
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="4"/>
+      <c r="A9" s="2"/>
       <c r="B9" s="1" t="s">
         <v>51</v>
       </c>
@@ -5306,7 +5010,7 @@
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="4"/>
+      <c r="A10" s="2"/>
       <c r="B10" s="1" t="s">
         <v>95</v>
       </c>
@@ -5316,7 +5020,7 @@
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B11" s="1"/>
@@ -5326,7 +5030,7 @@
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="4"/>
+      <c r="A12" s="2"/>
       <c r="B12" s="1" t="s">
         <v>96</v>
       </c>
@@ -5336,7 +5040,7 @@
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="4"/>
+      <c r="A13" s="2"/>
       <c r="B13" s="1" t="s">
         <v>97</v>
       </c>
@@ -5346,7 +5050,7 @@
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="4"/>
+      <c r="A14" s="2"/>
       <c r="B14" s="1" t="s">
         <v>98</v>
       </c>
@@ -5356,7 +5060,7 @@
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="4"/>
+      <c r="A15" s="2"/>
       <c r="B15" s="1" t="s">
         <v>99</v>
       </c>
@@ -5366,7 +5070,7 @@
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="4"/>
+      <c r="A16" s="2"/>
       <c r="B16" s="1" t="s">
         <v>100</v>
       </c>
@@ -5376,7 +5080,7 @@
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="4"/>
+      <c r="A17" s="2"/>
       <c r="B17" s="1" t="s">
         <v>101</v>
       </c>
@@ -5386,7 +5090,7 @@
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="4"/>
+      <c r="A18" s="2"/>
       <c r="B18" s="1" t="s">
         <v>102</v>
       </c>
@@ -5396,7 +5100,7 @@
       <c r="F18" s="1"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="4"/>
+      <c r="A19" s="2"/>
       <c r="B19" s="1" t="s">
         <v>103</v>
       </c>
@@ -5406,7 +5110,7 @@
       <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -5418,7 +5122,7 @@
       <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="4"/>
+      <c r="A21" s="2"/>
       <c r="B21" s="1" t="s">
         <v>16</v>
       </c>
@@ -5428,7 +5132,7 @@
       <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -5440,7 +5144,7 @@
       <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="4"/>
+      <c r="A23" s="2"/>
       <c r="B23" s="1" t="s">
         <v>19</v>
       </c>
@@ -5450,7 +5154,7 @@
       <c r="F23" s="1"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="4"/>
+      <c r="A24" s="2"/>
       <c r="B24" s="1" t="s">
         <v>20</v>
       </c>
@@ -5460,7 +5164,7 @@
       <c r="F24" s="1"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="4"/>
+      <c r="A25" s="2"/>
       <c r="B25" s="1" t="s">
         <v>21</v>
       </c>
@@ -5470,7 +5174,7 @@
       <c r="F25" s="1"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="4"/>
+      <c r="A26" s="2"/>
       <c r="B26" s="1" t="s">
         <v>22</v>
       </c>
@@ -5480,7 +5184,7 @@
       <c r="F26" s="1"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="4"/>
+      <c r="A27" s="2"/>
       <c r="B27" s="1" t="s">
         <v>23</v>
       </c>
@@ -5490,7 +5194,7 @@
       <c r="F27" s="1"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="4"/>
+      <c r="A28" s="2"/>
       <c r="B28" s="1" t="s">
         <v>24</v>
       </c>
@@ -5500,7 +5204,7 @@
       <c r="F28" s="1"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="4"/>
+      <c r="A29" s="2"/>
       <c r="B29" s="1" t="s">
         <v>25</v>
       </c>
@@ -5510,7 +5214,7 @@
       <c r="F29" s="1"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="4"/>
+      <c r="A30" s="2"/>
       <c r="B30" s="1" t="s">
         <v>26</v>
       </c>
@@ -5520,7 +5224,7 @@
       <c r="F30" s="1"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="4"/>
+      <c r="A31" s="2"/>
       <c r="B31" s="1" t="s">
         <v>27</v>
       </c>
@@ -5530,7 +5234,7 @@
       <c r="F31" s="1"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="4"/>
+      <c r="A32" s="2"/>
       <c r="B32" s="1" t="s">
         <v>28</v>
       </c>
@@ -5540,7 +5244,7 @@
       <c r="F32" s="1"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="4"/>
+      <c r="A33" s="2"/>
       <c r="B33" s="1" t="s">
         <v>29</v>
       </c>
@@ -5550,7 +5254,7 @@
       <c r="F33" s="1"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="4"/>
+      <c r="A34" s="2"/>
       <c r="B34" s="1" t="s">
         <v>30</v>
       </c>
@@ -5560,7 +5264,7 @@
       <c r="F34" s="1"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" s="4"/>
+      <c r="A35" s="2"/>
       <c r="B35" s="1" t="s">
         <v>31</v>
       </c>
@@ -5570,7 +5274,7 @@
       <c r="F35" s="1"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="4"/>
+      <c r="A36" s="2"/>
       <c r="B36" s="1" t="s">
         <v>32</v>
       </c>
@@ -5580,7 +5284,7 @@
       <c r="F36" s="1"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="4" t="s">
+      <c r="A37" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B37" s="1" t="s">
@@ -5592,7 +5296,7 @@
       <c r="F37" s="1"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="4"/>
+      <c r="A38" s="2"/>
       <c r="B38" s="1" t="s">
         <v>35</v>
       </c>
@@ -5602,7 +5306,7 @@
       <c r="F38" s="1"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="4"/>
+      <c r="A39" s="2"/>
       <c r="B39" s="1" t="s">
         <v>36</v>
       </c>
@@ -5612,7 +5316,7 @@
       <c r="F39" s="1"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="4"/>
+      <c r="A40" s="2"/>
       <c r="B40" s="1" t="s">
         <v>37</v>
       </c>
@@ -5622,7 +5326,7 @@
       <c r="F40" s="1"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" s="4"/>
+      <c r="A41" s="2"/>
       <c r="B41" s="1" t="s">
         <v>38</v>
       </c>
@@ -5632,7 +5336,7 @@
       <c r="F41" s="1"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" s="4"/>
+      <c r="A42" s="2"/>
       <c r="B42" s="1" t="s">
         <v>39</v>
       </c>
@@ -5642,7 +5346,7 @@
       <c r="F42" s="1"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="4"/>
+      <c r="A43" s="2"/>
       <c r="B43" s="1" t="s">
         <v>40</v>
       </c>
@@ -5652,7 +5356,7 @@
       <c r="F43" s="1"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" s="4"/>
+      <c r="A44" s="2"/>
       <c r="B44" s="1" t="s">
         <v>41</v>
       </c>
@@ -5662,7 +5366,7 @@
       <c r="F44" s="1"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" s="4"/>
+      <c r="A45" s="2"/>
       <c r="B45" s="1" t="s">
         <v>42</v>
       </c>
@@ -5672,7 +5376,7 @@
       <c r="F45" s="1"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" s="4"/>
+      <c r="A46" s="2"/>
       <c r="B46" s="1" t="s">
         <v>43</v>
       </c>
@@ -5682,7 +5386,7 @@
       <c r="F46" s="1"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" s="4"/>
+      <c r="A47" s="2"/>
       <c r="B47" s="1" t="s">
         <v>44</v>
       </c>
@@ -5692,7 +5396,7 @@
       <c r="F47" s="1"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48" s="4"/>
+      <c r="A48" s="2"/>
       <c r="B48" s="1" t="s">
         <v>45</v>
       </c>
@@ -5702,7 +5406,7 @@
       <c r="F48" s="1"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" s="4"/>
+      <c r="A49" s="2"/>
       <c r="B49" s="1" t="s">
         <v>46</v>
       </c>
@@ -5712,7 +5416,7 @@
       <c r="F49" s="1"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" s="4"/>
+      <c r="A50" s="2"/>
       <c r="B50" s="1" t="s">
         <v>47</v>
       </c>
@@ -5722,7 +5426,7 @@
       <c r="F50" s="1"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" s="4"/>
+      <c r="A51" s="2"/>
       <c r="B51" s="1" t="s">
         <v>48</v>
       </c>
@@ -5732,7 +5436,7 @@
       <c r="F51" s="1"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" s="4" t="s">
+      <c r="A52" s="2" t="s">
         <v>104</v>
       </c>
       <c r="B52" s="1" t="s">
@@ -5744,7 +5448,7 @@
       <c r="F52" s="1"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53" s="4"/>
+      <c r="A53" s="2"/>
       <c r="B53" s="1" t="s">
         <v>106</v>
       </c>
@@ -5754,7 +5458,7 @@
       <c r="F53" s="1"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A54" s="4"/>
+      <c r="A54" s="2"/>
       <c r="B54" s="1" t="s">
         <v>107</v>
       </c>
@@ -5764,7 +5468,7 @@
       <c r="F54" s="1"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A55" s="4"/>
+      <c r="A55" s="2"/>
       <c r="B55" s="1" t="s">
         <v>108</v>
       </c>
@@ -5774,7 +5478,7 @@
       <c r="F55" s="1"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A56" s="4"/>
+      <c r="A56" s="2"/>
       <c r="B56" s="1" t="s">
         <v>109</v>
       </c>
@@ -5784,7 +5488,7 @@
       <c r="F56" s="1"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A57" s="4"/>
+      <c r="A57" s="2"/>
       <c r="B57" s="1" t="s">
         <v>110</v>
       </c>
@@ -5794,7 +5498,7 @@
       <c r="F57" s="1"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A58" s="4"/>
+      <c r="A58" s="2"/>
       <c r="B58" s="1" t="s">
         <v>111</v>
       </c>
@@ -5804,7 +5508,7 @@
       <c r="F58" s="1"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59" s="4" t="s">
+      <c r="A59" s="2" t="s">
         <v>112</v>
       </c>
       <c r="B59" s="1" t="s">
@@ -5816,7 +5520,7 @@
       <c r="F59" s="1"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A60" s="4"/>
+      <c r="A60" s="2"/>
       <c r="B60" s="1" t="s">
         <v>114</v>
       </c>
@@ -5826,7 +5530,7 @@
       <c r="F60" s="1"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A61" s="4"/>
+      <c r="A61" s="2"/>
       <c r="B61" s="1" t="s">
         <v>115</v>
       </c>
@@ -5836,7 +5540,7 @@
       <c r="F61" s="1"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A62" s="4"/>
+      <c r="A62" s="2"/>
       <c r="B62" s="1" t="s">
         <v>116</v>
       </c>
@@ -5846,7 +5550,7 @@
       <c r="F62" s="1"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A63" s="4"/>
+      <c r="A63" s="2"/>
       <c r="B63" s="1" t="s">
         <v>117</v>
       </c>
@@ -5856,7 +5560,7 @@
       <c r="F63" s="1"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A64" s="4"/>
+      <c r="A64" s="2"/>
       <c r="B64" s="1" t="s">
         <v>118</v>
       </c>
@@ -5866,7 +5570,7 @@
       <c r="F64" s="1"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A65" s="4" t="s">
+      <c r="A65" s="2" t="s">
         <v>119</v>
       </c>
       <c r="B65" s="1" t="s">
@@ -5878,7 +5582,7 @@
       <c r="F65" s="1"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A66" s="4"/>
+      <c r="A66" s="2"/>
       <c r="B66" s="1" t="s">
         <v>114</v>
       </c>
@@ -5888,7 +5592,7 @@
       <c r="F66" s="1"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A67" s="4"/>
+      <c r="A67" s="2"/>
       <c r="B67" s="1" t="s">
         <v>115</v>
       </c>
@@ -5898,7 +5602,7 @@
       <c r="F67" s="1"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A68" s="4"/>
+      <c r="A68" s="2"/>
       <c r="B68" s="1" t="s">
         <v>116</v>
       </c>
@@ -5908,7 +5612,7 @@
       <c r="F68" s="1"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A69" s="4"/>
+      <c r="A69" s="2"/>
       <c r="B69" s="1" t="s">
         <v>117</v>
       </c>
@@ -5918,7 +5622,7 @@
       <c r="F69" s="1"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A70" s="4"/>
+      <c r="A70" s="2"/>
       <c r="B70" s="1" t="s">
         <v>118</v>
       </c>
@@ -5928,10 +5632,10 @@
       <c r="F70" s="1"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A71" s="4" t="s">
+      <c r="A71" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="B71" s="2" t="s">
         <v>121</v>
       </c>
       <c r="C71" s="1"/>
@@ -5940,15 +5644,15 @@
       <c r="F71" s="1"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A72" s="4"/>
-      <c r="B72" s="4"/>
+      <c r="A72" s="2"/>
+      <c r="B72" s="2"/>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
       <c r="F72" s="1"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A73" s="4"/>
+      <c r="A73" s="2"/>
       <c r="B73" s="1" t="s">
         <v>122</v>
       </c>
@@ -5958,7 +5662,7 @@
       <c r="F73" s="1"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A74" s="4"/>
+      <c r="A74" s="2"/>
       <c r="B74" s="1" t="s">
         <v>123</v>
       </c>
@@ -5968,7 +5672,7 @@
       <c r="F74" s="1"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A75" s="4"/>
+      <c r="A75" s="2"/>
       <c r="B75" s="1" t="s">
         <v>124</v>
       </c>
@@ -5978,7 +5682,7 @@
       <c r="F75" s="1"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A76" s="4"/>
+      <c r="A76" s="2"/>
       <c r="B76" s="1" t="s">
         <v>125</v>
       </c>
@@ -5988,7 +5692,7 @@
       <c r="F76" s="1"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A77" s="4"/>
+      <c r="A77" s="2"/>
       <c r="B77" s="1" t="s">
         <v>126</v>
       </c>
@@ -5998,10 +5702,10 @@
       <c r="F77" s="1"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A78" s="4" t="s">
+      <c r="A78" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B78" s="4" t="s">
+      <c r="B78" s="2" t="s">
         <v>121</v>
       </c>
       <c r="C78" s="1"/>
@@ -6010,15 +5714,15 @@
       <c r="F78" s="1"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A79" s="4"/>
-      <c r="B79" s="4"/>
+      <c r="A79" s="2"/>
+      <c r="B79" s="2"/>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
       <c r="E79" s="1"/>
       <c r="F79" s="1"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A80" s="4"/>
+      <c r="A80" s="2"/>
       <c r="B80" s="1" t="s">
         <v>122</v>
       </c>
@@ -6028,7 +5732,7 @@
       <c r="F80" s="1"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A81" s="4"/>
+      <c r="A81" s="2"/>
       <c r="B81" s="1" t="s">
         <v>123</v>
       </c>
@@ -6038,7 +5742,7 @@
       <c r="F81" s="1"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A82" s="4"/>
+      <c r="A82" s="2"/>
       <c r="B82" s="1" t="s">
         <v>124</v>
       </c>
@@ -6048,7 +5752,7 @@
       <c r="F82" s="1"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A83" s="4"/>
+      <c r="A83" s="2"/>
       <c r="B83" s="1" t="s">
         <v>125</v>
       </c>
@@ -6058,7 +5762,7 @@
       <c r="F83" s="1"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A84" s="4"/>
+      <c r="A84" s="2"/>
       <c r="B84" s="1" t="s">
         <v>126</v>
       </c>

</xml_diff>